<commit_message>
Hello World for Week 2 Studio
If we run uGrid_Net_LVMV_Reliability.py, we should be able to see some microgrid distribution layout iterating solutions starting at 60 poles, for the village of Ha Makebe.
</commit_message>
<xml_diff>
--- a/uGrid/uGrid_Input.xlsx
+++ b/uGrid/uGrid_Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phy\Documents\OnePower\Python Models Local Copy\uGrid-master-GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/cotillaj_oregonstate_edu/Documents/Teaching/ENGR100/Fall 21/Simulations/OnePower-Codes/uGrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FFA5B7-055B-494A-BC1D-A92FE2073C67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{32FFA5B7-055B-494A-BC1D-A92FE2073C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1CCC5F7-BC50-5C4F-80BC-26AF6F5CFF3F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="4" xr2:uid="{68709F03-E2F0-4CA3-951F-ABB4DD9E87C4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{68709F03-E2F0-4CA3-951F-ABB4DD9E87C4}"/>
   </bookViews>
   <sheets>
     <sheet name="PSO" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -639,29 +643,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810FAEA2-4EF8-4AD5-9CE0-4B60A3CE1971}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -708,9 +712,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -769,47 +773,47 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -928,7 +932,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>15</v>
       </c>
@@ -1049,7 +1053,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="O3" t="s">
         <v>67</v>
       </c>
@@ -1070,15 +1074,15 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1092,7 +1096,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1115,13 +1119,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26A88A2-799B-4631-B6FE-A8330968DD02}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1156,7 +1160,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2005</v>
       </c>
@@ -1200,28 +1204,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3256D70B-7508-42A8-AA62-A295C44165D1}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1262,7 +1266,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>

</xml_diff>